<commit_message>
Refactor pack EV calculation and Excel summary output; streamline data handling and improve formatting
</commit_message>
<xml_diff>
--- a/excelDocs/paradoxRift/pokemon_data.xlsx
+++ b/excelDocs/paradoxRift/pokemon_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2370" yWindow="2985" windowWidth="25260" windowHeight="11385" tabRatio="797" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-25665" yWindow="2085" windowWidth="25260" windowHeight="11880" tabRatio="797" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,9 +18,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <name val="Calibri"/>
@@ -141,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -170,22 +168,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -555,7 +541,7 @@
   </sheetPr>
   <dimension ref="A1:AY1263"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -573,8 +559,8 @@
     <col width="24" customWidth="1" min="10" max="10"/>
     <col width="15" customWidth="1" min="11" max="11"/>
     <col width="24" bestFit="1" customWidth="1" min="12" max="12"/>
-    <col width="20.4" customWidth="1" min="13" max="13"/>
-    <col width="28.8" customWidth="1" min="14" max="14"/>
+    <col width="20.42578125" customWidth="1" min="13" max="13"/>
+    <col width="28.85546875" customWidth="1" min="14" max="14"/>
     <col width="13.85546875" customWidth="1" min="15" max="15"/>
     <col width="33.5703125" customWidth="1" min="16" max="16"/>
     <col width="26.85546875" customWidth="1" min="17" max="17"/>
@@ -587,7 +573,7 @@
     <col width="24" customWidth="1" min="48" max="48"/>
     <col width="20.42578125" customWidth="1" min="49" max="49"/>
     <col width="28.85546875" customWidth="1" min="50" max="50"/>
-    <col width="16.8" customWidth="1" min="51" max="51"/>
+    <col width="16.85546875" customWidth="1" min="51" max="51"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -854,7 +840,7 @@
       <c r="D4" s="3" t="n">
         <v>5.77</v>
       </c>
-      <c r="E4" s="3" t="inlineStr"/>
+      <c r="E4" s="3" t="n"/>
       <c r="F4" s="3">
         <f>IF(B4="common", 4, IF(B4="uncommon", 3, IF(B4="rare", 0.73878, 1)))</f>
         <v/>
@@ -913,7 +899,7 @@
       <c r="D5" s="3" t="n">
         <v>0.59</v>
       </c>
-      <c r="E5" s="3" t="inlineStr"/>
+      <c r="E5" s="3" t="n"/>
       <c r="F5" s="3">
         <f>IF(B5="common", 4, IF(B5="uncommon", 3, IF(B5="rare", 0.73878, 1)))</f>
         <v/>
@@ -972,7 +958,7 @@
       <c r="D6" s="3" t="n">
         <v>1.5</v>
       </c>
-      <c r="E6" s="3" t="inlineStr"/>
+      <c r="E6" s="3" t="n"/>
       <c r="F6" s="3">
         <f>IF(B6="common", 4, IF(B6="uncommon", 3, IF(B6="rare", 0.73878, 1)))</f>
         <v/>
@@ -1092,7 +1078,7 @@
       <c r="D8" s="3" t="n">
         <v>7.19</v>
       </c>
-      <c r="E8" s="3" t="inlineStr"/>
+      <c r="E8" s="3" t="n"/>
       <c r="F8" s="3">
         <f>IF(B8="common", 4, IF(B8="uncommon", 3, IF(B8="rare", 0.73878, 1)))</f>
         <v/>
@@ -1151,7 +1137,7 @@
       <c r="D9" s="3" t="n">
         <v>0.72</v>
       </c>
-      <c r="E9" s="3" t="inlineStr"/>
+      <c r="E9" s="3" t="n"/>
       <c r="F9" s="3">
         <f>IF(B9="common", 4, IF(B9="uncommon", 3, IF(B9="rare", 0.73878, 1)))</f>
         <v/>
@@ -1210,7 +1196,7 @@
       <c r="D10" s="3" t="n">
         <v>2.29</v>
       </c>
-      <c r="E10" s="3" t="inlineStr"/>
+      <c r="E10" s="3" t="n"/>
       <c r="F10" s="3">
         <f>IF(B10="common", 4, IF(B10="uncommon", 3, IF(B10="rare", 0.73878, 1)))</f>
         <v/>
@@ -1269,7 +1255,7 @@
       <c r="D11" s="3" t="n">
         <v>43.83</v>
       </c>
-      <c r="E11" s="3" t="inlineStr"/>
+      <c r="E11" s="3" t="n"/>
       <c r="F11" s="3">
         <f>IF(B11="common", 4, IF(B11="uncommon", 3, IF(B11="rare", 0.73878, 1)))</f>
         <v/>
@@ -1454,7 +1440,7 @@
       <c r="D14" s="3" t="n">
         <v>0.63</v>
       </c>
-      <c r="E14" s="3" t="inlineStr"/>
+      <c r="E14" s="3" t="n"/>
       <c r="F14" s="3">
         <f>IF(B14="common", 4, IF(B14="uncommon", 3, IF(B14="rare", 0.73878, 1)))</f>
         <v/>
@@ -1510,7 +1496,7 @@
       <c r="D15" s="3" t="n">
         <v>1.69</v>
       </c>
-      <c r="E15" s="3" t="inlineStr"/>
+      <c r="E15" s="3" t="n"/>
       <c r="F15" s="3">
         <f>IF(B15="common", 4, IF(B15="uncommon", 3, IF(B15="rare", 0.73878, 1)))</f>
         <v/>
@@ -1566,7 +1552,7 @@
       <c r="D16" s="3" t="n">
         <v>2.89</v>
       </c>
-      <c r="E16" s="3" t="inlineStr"/>
+      <c r="E16" s="3" t="n"/>
       <c r="F16" s="3">
         <f>IF(B16="common", 4, IF(B16="uncommon", 3, IF(B16="rare", 0.73878, 1)))</f>
         <v/>
@@ -1741,7 +1727,7 @@
       <c r="D19" s="3" t="n">
         <v>5.68</v>
       </c>
-      <c r="E19" s="3" t="inlineStr"/>
+      <c r="E19" s="3" t="n"/>
       <c r="F19" s="3">
         <f>IF(B19="common", 4, IF(B19="uncommon", 3, IF(B19="rare", 0.73878, 1)))</f>
         <v/>
@@ -1797,7 +1783,7 @@
       <c r="D20" s="3" t="n">
         <v>0.57</v>
       </c>
-      <c r="E20" s="3" t="inlineStr"/>
+      <c r="E20" s="3" t="n"/>
       <c r="F20" s="3">
         <f>IF(B20="common", 4, IF(B20="uncommon", 3, IF(B20="rare", 0.73878, 1)))</f>
         <v/>
@@ -1853,7 +1839,7 @@
       <c r="D21" s="3" t="n">
         <v>1.46</v>
       </c>
-      <c r="E21" s="3" t="inlineStr"/>
+      <c r="E21" s="3" t="n"/>
       <c r="F21" s="3">
         <f>IF(B21="common", 4, IF(B21="uncommon", 3, IF(B21="rare", 0.73878, 1)))</f>
         <v/>
@@ -2034,7 +2020,7 @@
       <c r="D24" s="3" t="n">
         <v>7.71</v>
       </c>
-      <c r="E24" s="3" t="inlineStr"/>
+      <c r="E24" s="3" t="n"/>
       <c r="F24" s="3">
         <f>IF(B24="common", 4, IF(B24="uncommon", 3, IF(B24="rare", 0.73878, 1)))</f>
         <v/>
@@ -2322,7 +2308,7 @@
       <c r="D29" s="3" t="n">
         <v>0.48</v>
       </c>
-      <c r="E29" s="3" t="inlineStr"/>
+      <c r="E29" s="3" t="n"/>
       <c r="F29" s="3">
         <f>IF(B29="common", 4, IF(B29="uncommon", 3, IF(B29="rare", 0.73878, 1)))</f>
         <v/>
@@ -2378,7 +2364,7 @@
       <c r="D30" s="3" t="n">
         <v>1.68</v>
       </c>
-      <c r="E30" s="3" t="inlineStr"/>
+      <c r="E30" s="3" t="n"/>
       <c r="F30" s="3">
         <f>IF(B30="common", 4, IF(B30="uncommon", 3, IF(B30="rare", 0.73878, 1)))</f>
         <v/>
@@ -2492,7 +2478,7 @@
       <c r="D32" s="3" t="n">
         <v>6.56</v>
       </c>
-      <c r="E32" s="3" t="inlineStr"/>
+      <c r="E32" s="3" t="n"/>
       <c r="F32" s="3">
         <f>IF(B32="common", 4, IF(B32="uncommon", 3, IF(B32="rare", 0.73878, 1)))</f>
         <v/>
@@ -2722,7 +2708,7 @@
       <c r="D36" s="3" t="n">
         <v>3.39</v>
       </c>
-      <c r="E36" s="3" t="inlineStr"/>
+      <c r="E36" s="3" t="n"/>
       <c r="F36" s="3">
         <f>IF(B36="common", 4, IF(B36="uncommon", 3, IF(B36="rare", 0.73878, 1)))</f>
         <v/>
@@ -2894,7 +2880,7 @@
       <c r="D39" s="3" t="n">
         <v>3.76</v>
       </c>
-      <c r="E39" s="3" t="inlineStr"/>
+      <c r="E39" s="3" t="n"/>
       <c r="F39" s="3">
         <f>IF(B39="common", 4, IF(B39="uncommon", 3, IF(B39="rare", 0.73878, 1)))</f>
         <v/>
@@ -3182,7 +3168,7 @@
       <c r="D44" s="3" t="n">
         <v>2.98</v>
       </c>
-      <c r="E44" s="3" t="inlineStr"/>
+      <c r="E44" s="3" t="n"/>
       <c r="F44" s="3">
         <f>IF(B44="common", 4, IF(B44="uncommon", 3, IF(B44="rare", 0.73878, 1)))</f>
         <v/>
@@ -3644,7 +3630,7 @@
       <c r="D52" s="3" t="n">
         <v>5.53</v>
       </c>
-      <c r="E52" s="3" t="inlineStr"/>
+      <c r="E52" s="3" t="n"/>
       <c r="F52" s="3">
         <f>IF(B52="common", 4, IF(B52="uncommon", 3, IF(B52="rare", 0.73878, 1)))</f>
         <v/>
@@ -3932,7 +3918,7 @@
       <c r="D57" s="3" t="n">
         <v>4.33</v>
       </c>
-      <c r="E57" s="3" t="inlineStr"/>
+      <c r="E57" s="3" t="n"/>
       <c r="F57" s="3">
         <f>IF(B57="common", 4, IF(B57="uncommon", 3, IF(B57="rare", 0.73878, 1)))</f>
         <v/>
@@ -4162,7 +4148,7 @@
       <c r="D61" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="E61" s="3" t="inlineStr"/>
+      <c r="E61" s="3" t="n"/>
       <c r="F61" s="3">
         <f>IF(B61="common", 4, IF(B61="uncommon", 3, IF(B61="rare", 0.73878, 1)))</f>
         <v/>
@@ -4218,7 +4204,7 @@
       <c r="D62" s="3" t="n">
         <v>1.78</v>
       </c>
-      <c r="E62" s="3" t="inlineStr"/>
+      <c r="E62" s="3" t="n"/>
       <c r="F62" s="3">
         <f>IF(B62="common", 4, IF(B62="uncommon", 3, IF(B62="rare", 0.73878, 1)))</f>
         <v/>
@@ -4564,7 +4550,7 @@
       <c r="D68" s="3" t="n">
         <v>8.33</v>
       </c>
-      <c r="E68" s="3" t="inlineStr"/>
+      <c r="E68" s="3" t="n"/>
       <c r="F68" s="3">
         <f>IF(B68="common", 4, IF(B68="uncommon", 3, IF(B68="rare", 0.73878, 1)))</f>
         <v/>
@@ -4620,7 +4606,7 @@
       <c r="D69" s="3" t="n">
         <v>0.76</v>
       </c>
-      <c r="E69" s="3" t="inlineStr"/>
+      <c r="E69" s="3" t="n"/>
       <c r="F69" s="3">
         <f>IF(B69="common", 4, IF(B69="uncommon", 3, IF(B69="rare", 0.73878, 1)))</f>
         <v/>
@@ -4676,7 +4662,7 @@
       <c r="D70" s="3" t="n">
         <v>5.86</v>
       </c>
-      <c r="E70" s="3" t="inlineStr"/>
+      <c r="E70" s="3" t="n"/>
       <c r="F70" s="3">
         <f>IF(B70="common", 4, IF(B70="uncommon", 3, IF(B70="rare", 0.73878, 1)))</f>
         <v/>
@@ -4732,7 +4718,7 @@
       <c r="D71" s="3" t="n">
         <v>34.59</v>
       </c>
-      <c r="E71" s="3" t="inlineStr"/>
+      <c r="E71" s="3" t="n"/>
       <c r="F71" s="3">
         <f>IF(B71="common", 4, IF(B71="uncommon", 3, IF(B71="rare", 0.73878, 1)))</f>
         <v/>
@@ -4788,7 +4774,7 @@
       <c r="D72" s="3" t="n">
         <v>10.14</v>
       </c>
-      <c r="E72" s="3" t="inlineStr"/>
+      <c r="E72" s="3" t="n"/>
       <c r="F72" s="3">
         <f>IF(B72="common", 4, IF(B72="uncommon", 3, IF(B72="rare", 0.73878, 1)))</f>
         <v/>
@@ -4902,7 +4888,7 @@
       <c r="D74" s="3" t="n">
         <v>4.02</v>
       </c>
-      <c r="E74" s="3" t="inlineStr"/>
+      <c r="E74" s="3" t="n"/>
       <c r="F74" s="3">
         <f>IF(B74="common", 4, IF(B74="uncommon", 3, IF(B74="rare", 0.73878, 1)))</f>
         <v/>
@@ -4958,7 +4944,7 @@
       <c r="D75" s="3" t="n">
         <v>12.66</v>
       </c>
-      <c r="E75" s="3" t="inlineStr"/>
+      <c r="E75" s="3" t="n"/>
       <c r="F75" s="3">
         <f>IF(B75="common", 4, IF(B75="uncommon", 3, IF(B75="rare", 0.73878, 1)))</f>
         <v/>
@@ -5014,7 +5000,7 @@
       <c r="D76" s="3" t="n">
         <v>14.18</v>
       </c>
-      <c r="E76" s="3" t="inlineStr"/>
+      <c r="E76" s="3" t="n"/>
       <c r="F76" s="3">
         <f>IF(B76="common", 4, IF(B76="uncommon", 3, IF(B76="rare", 0.73878, 1)))</f>
         <v/>
@@ -5070,7 +5056,7 @@
       <c r="D77" s="3" t="n">
         <v>29.93</v>
       </c>
-      <c r="E77" s="3" t="inlineStr"/>
+      <c r="E77" s="3" t="n"/>
       <c r="F77" s="3">
         <f>IF(B77="common", 4, IF(B77="uncommon", 3, IF(B77="rare", 0.73878, 1)))</f>
         <v/>
@@ -5300,7 +5286,7 @@
       <c r="D81" s="3" t="n">
         <v>12.71</v>
       </c>
-      <c r="E81" s="3" t="inlineStr"/>
+      <c r="E81" s="3" t="n"/>
       <c r="F81" s="3">
         <f>IF(B81="common", 4, IF(B81="uncommon", 3, IF(B81="rare", 0.73878, 1)))</f>
         <v/>
@@ -5588,7 +5574,7 @@
       <c r="D86" s="3" t="n">
         <v>0.52</v>
       </c>
-      <c r="E86" s="3" t="inlineStr"/>
+      <c r="E86" s="3" t="n"/>
       <c r="F86" s="3">
         <f>IF(B86="common", 4, IF(B86="uncommon", 3, IF(B86="rare", 0.73878, 1)))</f>
         <v/>
@@ -5644,7 +5630,7 @@
       <c r="D87" s="3" t="n">
         <v>1.66</v>
       </c>
-      <c r="E87" s="3" t="inlineStr"/>
+      <c r="E87" s="3" t="n"/>
       <c r="F87" s="3">
         <f>IF(B87="common", 4, IF(B87="uncommon", 3, IF(B87="rare", 0.73878, 1)))</f>
         <v/>
@@ -5700,7 +5686,7 @@
       <c r="D88" s="3" t="n">
         <v>15.91</v>
       </c>
-      <c r="E88" s="3" t="inlineStr"/>
+      <c r="E88" s="3" t="n"/>
       <c r="F88" s="3">
         <f>IF(B88="common", 4, IF(B88="uncommon", 3, IF(B88="rare", 0.73878, 1)))</f>
         <v/>
@@ -5872,7 +5858,7 @@
       <c r="D91" s="3" t="n">
         <v>91.09</v>
       </c>
-      <c r="E91" s="3" t="inlineStr"/>
+      <c r="E91" s="3" t="n"/>
       <c r="F91" s="3">
         <f>IF(B91="common", 4, IF(B91="uncommon", 3, IF(B91="rare", 0.73878, 1)))</f>
         <v/>
@@ -6044,7 +6030,7 @@
       <c r="D94" s="3" t="n">
         <v>0.5600000000000001</v>
       </c>
-      <c r="E94" s="3" t="inlineStr"/>
+      <c r="E94" s="3" t="n"/>
       <c r="F94" s="3">
         <f>IF(B94="common", 4, IF(B94="uncommon", 3, IF(B94="rare", 0.73878, 1)))</f>
         <v/>
@@ -6100,7 +6086,7 @@
       <c r="D95" s="3" t="n">
         <v>2.59</v>
       </c>
-      <c r="E95" s="3" t="inlineStr"/>
+      <c r="E95" s="3" t="n"/>
       <c r="F95" s="3">
         <f>IF(B95="common", 4, IF(B95="uncommon", 3, IF(B95="rare", 0.73878, 1)))</f>
         <v/>
@@ -6272,7 +6258,7 @@
       <c r="D98" s="3" t="n">
         <v>1.32</v>
       </c>
-      <c r="E98" s="3" t="inlineStr"/>
+      <c r="E98" s="3" t="n"/>
       <c r="F98" s="3">
         <f>IF(B98="common", 4, IF(B98="uncommon", 3, IF(B98="rare", 0.73878, 1)))</f>
         <v/>
@@ -6328,7 +6314,7 @@
       <c r="D99" s="3" t="n">
         <v>4.42</v>
       </c>
-      <c r="E99" s="3" t="inlineStr"/>
+      <c r="E99" s="3" t="n"/>
       <c r="F99" s="3">
         <f>IF(B99="common", 4, IF(B99="uncommon", 3, IF(B99="rare", 0.73878, 1)))</f>
         <v/>
@@ -6384,7 +6370,7 @@
       <c r="D100" s="3" t="n">
         <v>13.62</v>
       </c>
-      <c r="E100" s="3" t="inlineStr"/>
+      <c r="E100" s="3" t="n"/>
       <c r="F100" s="3">
         <f>IF(B100="common", 4, IF(B100="uncommon", 3, IF(B100="rare", 0.73878, 1)))</f>
         <v/>
@@ -6498,7 +6484,7 @@
       <c r="D102" s="3" t="n">
         <v>6.29</v>
       </c>
-      <c r="E102" s="3" t="inlineStr"/>
+      <c r="E102" s="3" t="n"/>
       <c r="F102" s="3">
         <f>IF(B102="common", 4, IF(B102="uncommon", 3, IF(B102="rare", 0.73878, 1)))</f>
         <v/>
@@ -6612,7 +6598,7 @@
       <c r="D104" s="3" t="n">
         <v>4.71</v>
       </c>
-      <c r="E104" s="3" t="inlineStr"/>
+      <c r="E104" s="3" t="n"/>
       <c r="F104" s="3">
         <f>IF(B104="common", 4, IF(B104="uncommon", 3, IF(B104="rare", 0.73878, 1)))</f>
         <v/>
@@ -6668,7 +6654,7 @@
       <c r="D105" s="3" t="n">
         <v>0.57</v>
       </c>
-      <c r="E105" s="3" t="inlineStr"/>
+      <c r="E105" s="3" t="n"/>
       <c r="F105" s="3">
         <f>IF(B105="common", 4, IF(B105="uncommon", 3, IF(B105="rare", 0.73878, 1)))</f>
         <v/>
@@ -6724,7 +6710,7 @@
       <c r="D106" s="3" t="n">
         <v>2.56</v>
       </c>
-      <c r="E106" s="3" t="inlineStr"/>
+      <c r="E106" s="3" t="n"/>
       <c r="F106" s="3">
         <f>IF(B106="common", 4, IF(B106="uncommon", 3, IF(B106="rare", 0.73878, 1)))</f>
         <v/>
@@ -6780,7 +6766,7 @@
       <c r="D107" s="3" t="n">
         <v>23.01</v>
       </c>
-      <c r="E107" s="3" t="inlineStr"/>
+      <c r="E107" s="3" t="n"/>
       <c r="F107" s="3">
         <f>IF(B107="common", 4, IF(B107="uncommon", 3, IF(B107="rare", 0.73878, 1)))</f>
         <v/>
@@ -6836,7 +6822,7 @@
       <c r="D108" s="3" t="n">
         <v>4.43</v>
       </c>
-      <c r="E108" s="3" t="inlineStr"/>
+      <c r="E108" s="3" t="n"/>
       <c r="F108" s="3">
         <f>IF(B108="common", 4, IF(B108="uncommon", 3, IF(B108="rare", 0.73878, 1)))</f>
         <v/>
@@ -7008,7 +6994,7 @@
       <c r="D111" s="3" t="n">
         <v>10.11</v>
       </c>
-      <c r="E111" s="3" t="inlineStr"/>
+      <c r="E111" s="3" t="n"/>
       <c r="F111" s="3">
         <f>IF(B111="common", 4, IF(B111="uncommon", 3, IF(B111="rare", 0.73878, 1)))</f>
         <v/>
@@ -7238,7 +7224,7 @@
       <c r="D115" s="3" t="n">
         <v>1.7</v>
       </c>
-      <c r="E115" s="3" t="inlineStr"/>
+      <c r="E115" s="3" t="n"/>
       <c r="F115" s="3">
         <f>IF(B115="common", 4, IF(B115="uncommon", 3, IF(B115="rare", 0.73878, 1)))</f>
         <v/>
@@ -7526,7 +7512,7 @@
       <c r="D120" s="3" t="n">
         <v>11.37</v>
       </c>
-      <c r="E120" s="3" t="inlineStr"/>
+      <c r="E120" s="3" t="n"/>
       <c r="F120" s="3">
         <f>IF(B120="common", 4, IF(B120="uncommon", 3, IF(B120="rare", 0.73878, 1)))</f>
         <v/>
@@ -7640,7 +7626,7 @@
       <c r="D122" s="3" t="n">
         <v>3.52</v>
       </c>
-      <c r="E122" s="3" t="inlineStr"/>
+      <c r="E122" s="3" t="n"/>
       <c r="F122" s="3">
         <f>IF(B122="common", 4, IF(B122="uncommon", 3, IF(B122="rare", 0.73878, 1)))</f>
         <v/>
@@ -7754,7 +7740,7 @@
       <c r="D124" s="3" t="n">
         <v>11.87</v>
       </c>
-      <c r="E124" s="3" t="inlineStr"/>
+      <c r="E124" s="3" t="n"/>
       <c r="F124" s="3">
         <f>IF(B124="common", 4, IF(B124="uncommon", 3, IF(B124="rare", 0.73878, 1)))</f>
         <v/>
@@ -7868,7 +7854,7 @@
       <c r="D126" s="3" t="n">
         <v>16.51</v>
       </c>
-      <c r="E126" s="3" t="inlineStr"/>
+      <c r="E126" s="3" t="n"/>
       <c r="F126" s="3">
         <f>IF(B126="common", 4, IF(B126="uncommon", 3, IF(B126="rare", 0.73878, 1)))</f>
         <v/>
@@ -7982,7 +7968,7 @@
       <c r="D128" s="3" t="n">
         <v>0.6899999999999999</v>
       </c>
-      <c r="E128" s="3" t="inlineStr"/>
+      <c r="E128" s="3" t="n"/>
       <c r="F128" s="3">
         <f>IF(B128="common", 4, IF(B128="uncommon", 3, IF(B128="rare", 0.73878, 1)))</f>
         <v/>
@@ -8038,7 +8024,7 @@
       <c r="D129" s="3" t="n">
         <v>7.62</v>
       </c>
-      <c r="E129" s="3" t="inlineStr"/>
+      <c r="E129" s="3" t="n"/>
       <c r="F129" s="3">
         <f>IF(B129="common", 4, IF(B129="uncommon", 3, IF(B129="rare", 0.73878, 1)))</f>
         <v/>
@@ -8210,7 +8196,7 @@
       <c r="D132" s="3" t="n">
         <v>2.17</v>
       </c>
-      <c r="E132" s="3" t="inlineStr"/>
+      <c r="E132" s="3" t="n"/>
       <c r="F132" s="3">
         <f>IF(B132="common", 4, IF(B132="uncommon", 3, IF(B132="rare", 0.73878, 1)))</f>
         <v/>
@@ -8266,7 +8252,7 @@
       <c r="D133" s="3" t="n">
         <v>7.56</v>
       </c>
-      <c r="E133" s="3" t="inlineStr"/>
+      <c r="E133" s="3" t="n"/>
       <c r="F133" s="3">
         <f>IF(B133="common", 4, IF(B133="uncommon", 3, IF(B133="rare", 0.73878, 1)))</f>
         <v/>
@@ -8322,7 +8308,7 @@
       <c r="D134" s="3" t="n">
         <v>1.36</v>
       </c>
-      <c r="E134" s="3" t="inlineStr"/>
+      <c r="E134" s="3" t="n"/>
       <c r="F134" s="3">
         <f>IF(B134="common", 4, IF(B134="uncommon", 3, IF(B134="rare", 0.73878, 1)))</f>
         <v/>
@@ -8494,7 +8480,7 @@
       <c r="D137" s="3" t="n">
         <v>6.6</v>
       </c>
-      <c r="E137" s="3" t="inlineStr"/>
+      <c r="E137" s="3" t="n"/>
       <c r="F137" s="3">
         <f>IF(B137="common", 4, IF(B137="uncommon", 3, IF(B137="rare", 0.73878, 1)))</f>
         <v/>
@@ -8724,7 +8710,7 @@
       <c r="D141" s="3" t="n">
         <v>12.65</v>
       </c>
-      <c r="E141" s="3" t="inlineStr"/>
+      <c r="E141" s="3" t="n"/>
       <c r="F141" s="3">
         <f>IF(B141="common", 4, IF(B141="uncommon", 3, IF(B141="rare", 0.73878, 1)))</f>
         <v/>
@@ -8838,7 +8824,7 @@
       <c r="D143" s="3" t="n">
         <v>22.43</v>
       </c>
-      <c r="E143" s="3" t="inlineStr"/>
+      <c r="E143" s="3" t="n"/>
       <c r="F143" s="3">
         <f>IF(B143="common", 4, IF(B143="uncommon", 3, IF(B143="rare", 0.73878, 1)))</f>
         <v/>
@@ -8952,7 +8938,7 @@
       <c r="D145" s="3" t="n">
         <v>20.49</v>
       </c>
-      <c r="E145" s="3" t="inlineStr"/>
+      <c r="E145" s="3" t="n"/>
       <c r="F145" s="3">
         <f>IF(B145="common", 4, IF(B145="uncommon", 3, IF(B145="rare", 0.73878, 1)))</f>
         <v/>
@@ -9356,7 +9342,7 @@
       <c r="D152" s="3" t="n">
         <v>1.29</v>
       </c>
-      <c r="E152" s="3" t="inlineStr"/>
+      <c r="E152" s="3" t="n"/>
       <c r="F152" s="3">
         <f>IF(B152="common", 4, IF(B152="uncommon", 3, IF(B152="rare", 0.73878, 1)))</f>
         <v/>
@@ -10108,7 +10094,7 @@
       <c r="D165" s="3" t="n">
         <v>3.91</v>
       </c>
-      <c r="E165" s="3" t="inlineStr"/>
+      <c r="E165" s="3" t="n"/>
       <c r="F165" s="3">
         <f>IF(B165="common", 4, IF(B165="uncommon", 3, IF(B165="rare", 0.73878, 1)))</f>
         <v/>
@@ -10164,7 +10150,7 @@
       <c r="D166" s="3" t="n">
         <v>12.36</v>
       </c>
-      <c r="E166" s="3" t="inlineStr"/>
+      <c r="E166" s="3" t="n"/>
       <c r="F166" s="3">
         <f>IF(B166="common", 4, IF(B166="uncommon", 3, IF(B166="rare", 0.73878, 1)))</f>
         <v/>
@@ -10278,7 +10264,7 @@
       <c r="D168" s="3" t="n">
         <v>20.85</v>
       </c>
-      <c r="E168" s="3" t="inlineStr"/>
+      <c r="E168" s="3" t="n"/>
       <c r="F168" s="3">
         <f>IF(B168="common", 4, IF(B168="uncommon", 3, IF(B168="rare", 0.73878, 1)))</f>
         <v/>
@@ -10450,7 +10436,7 @@
       <c r="D171" s="3" t="n">
         <v>7.5</v>
       </c>
-      <c r="E171" s="3" t="inlineStr"/>
+      <c r="E171" s="3" t="n"/>
       <c r="F171" s="3">
         <f>IF(B171="common", 4, IF(B171="uncommon", 3, IF(B171="rare", 0.73878, 1)))</f>
         <v/>
@@ -10622,7 +10608,7 @@
       <c r="D174" s="3" t="n">
         <v>4.4</v>
       </c>
-      <c r="E174" s="3" t="inlineStr"/>
+      <c r="E174" s="3" t="n"/>
       <c r="F174" s="3">
         <f>IF(B174="common", 4, IF(B174="uncommon", 3, IF(B174="rare", 0.73878, 1)))</f>
         <v/>
@@ -10678,7 +10664,7 @@
       <c r="D175" s="3" t="n">
         <v>10.66</v>
       </c>
-      <c r="E175" s="3" t="inlineStr"/>
+      <c r="E175" s="3" t="n"/>
       <c r="F175" s="3">
         <f>IF(B175="common", 4, IF(B175="uncommon", 3, IF(B175="rare", 0.73878, 1)))</f>
         <v/>
@@ -10792,7 +10778,7 @@
       <c r="D177" s="3" t="n">
         <v>3.76</v>
       </c>
-      <c r="E177" s="3" t="inlineStr"/>
+      <c r="E177" s="3" t="n"/>
       <c r="F177" s="3">
         <f>IF(B177="common", 4, IF(B177="uncommon", 3, IF(B177="rare", 0.73878, 1)))</f>
         <v/>
@@ -10848,7 +10834,7 @@
       <c r="D178" s="3" t="n">
         <v>8.109999999999999</v>
       </c>
-      <c r="E178" s="3" t="inlineStr"/>
+      <c r="E178" s="3" t="n"/>
       <c r="F178" s="3">
         <f>IF(B178="common", 4, IF(B178="uncommon", 3, IF(B178="rare", 0.73878, 1)))</f>
         <v/>
@@ -11078,7 +11064,7 @@
       <c r="D182" s="3" t="n">
         <v>4.35</v>
       </c>
-      <c r="E182" s="3" t="inlineStr"/>
+      <c r="E182" s="3" t="n"/>
       <c r="F182" s="3">
         <f>IF(B182="common", 4, IF(B182="uncommon", 3, IF(B182="rare", 0.73878, 1)))</f>
         <v/>
@@ -11192,7 +11178,7 @@
       <c r="D184" s="3" t="n">
         <v>2.36</v>
       </c>
-      <c r="E184" s="3" t="inlineStr"/>
+      <c r="E184" s="3" t="n"/>
       <c r="F184" s="3">
         <f>IF(B184="common", 4, IF(B184="uncommon", 3, IF(B184="rare", 0.73878, 1)))</f>
         <v/>
@@ -11248,7 +11234,7 @@
       <c r="D185" s="3" t="n">
         <v>7.31</v>
       </c>
-      <c r="E185" s="3" t="inlineStr"/>
+      <c r="E185" s="3" t="n"/>
       <c r="F185" s="3">
         <f>IF(B185="common", 4, IF(B185="uncommon", 3, IF(B185="rare", 0.73878, 1)))</f>
         <v/>
@@ -11304,7 +11290,7 @@
       <c r="D186" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="E186" s="3" t="inlineStr"/>
+      <c r="E186" s="3" t="n"/>
       <c r="F186" s="3">
         <f>IF(B186="common", 4, IF(B186="uncommon", 3, IF(B186="rare", 0.73878, 1)))</f>
         <v/>
@@ -11360,7 +11346,7 @@
       <c r="D187" s="3" t="n">
         <v>3.41</v>
       </c>
-      <c r="E187" s="3" t="inlineStr"/>
+      <c r="E187" s="3" t="n"/>
       <c r="F187" s="3">
         <f>IF(B187="common", 4, IF(B187="uncommon", 3, IF(B187="rare", 0.73878, 1)))</f>
         <v/>
@@ -11416,7 +11402,7 @@
       <c r="D188" s="3" t="n">
         <v>43.85</v>
       </c>
-      <c r="E188" s="3" t="inlineStr"/>
+      <c r="E188" s="3" t="n"/>
       <c r="F188" s="3">
         <f>IF(B188="common", 4, IF(B188="uncommon", 3, IF(B188="rare", 0.73878, 1)))</f>
         <v/>
@@ -11472,7 +11458,7 @@
       <c r="D189" s="3" t="n">
         <v>6.21</v>
       </c>
-      <c r="E189" s="3" t="inlineStr"/>
+      <c r="E189" s="3" t="n"/>
       <c r="F189" s="3">
         <f>IF(B189="common", 4, IF(B189="uncommon", 3, IF(B189="rare", 0.73878, 1)))</f>
         <v/>
@@ -11586,7 +11572,7 @@
       <c r="D191" s="3" t="n">
         <v>1.43</v>
       </c>
-      <c r="E191" s="3" t="inlineStr"/>
+      <c r="E191" s="3" t="n"/>
       <c r="F191" s="3">
         <f>IF(B191="common", 4, IF(B191="uncommon", 3, IF(B191="rare", 0.73878, 1)))</f>
         <v/>
@@ -11642,7 +11628,7 @@
       <c r="D192" s="3" t="n">
         <v>0.5</v>
       </c>
-      <c r="E192" s="3" t="inlineStr"/>
+      <c r="E192" s="3" t="n"/>
       <c r="F192" s="3">
         <f>IF(B192="common", 4, IF(B192="uncommon", 3, IF(B192="rare", 0.73878, 1)))</f>
         <v/>
@@ -11698,7 +11684,7 @@
       <c r="D193" s="3" t="n">
         <v>1.66</v>
       </c>
-      <c r="E193" s="3" t="inlineStr"/>
+      <c r="E193" s="3" t="n"/>
       <c r="F193" s="3">
         <f>IF(B193="common", 4, IF(B193="uncommon", 3, IF(B193="rare", 0.73878, 1)))</f>
         <v/>
@@ -11754,7 +11740,7 @@
       <c r="D194" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="E194" s="3" t="inlineStr"/>
+      <c r="E194" s="3" t="n"/>
       <c r="F194" s="3">
         <f>IF(B194="common", 4, IF(B194="uncommon", 3, IF(B194="rare", 0.73878, 1)))</f>
         <v/>
@@ -11984,7 +11970,7 @@
       <c r="D198" s="3" t="n">
         <v>2.2</v>
       </c>
-      <c r="E198" s="3" t="inlineStr"/>
+      <c r="E198" s="3" t="n"/>
       <c r="F198" s="3">
         <f>IF(B198="common", 4, IF(B198="uncommon", 3, IF(B198="rare", 0.73878, 1)))</f>
         <v/>
@@ -12214,7 +12200,7 @@
       <c r="D202" s="3" t="n">
         <v>0.71</v>
       </c>
-      <c r="E202" s="3" t="inlineStr"/>
+      <c r="E202" s="3" t="n"/>
       <c r="F202" s="3">
         <f>IF(B202="common", 4, IF(B202="uncommon", 3, IF(B202="rare", 0.73878, 1)))</f>
         <v/>
@@ -12328,7 +12314,7 @@
       <c r="D204" s="3" t="n">
         <v>4.38</v>
       </c>
-      <c r="E204" s="3" t="inlineStr"/>
+      <c r="E204" s="3" t="n"/>
       <c r="F204" s="3">
         <f>IF(B204="common", 4, IF(B204="uncommon", 3, IF(B204="rare", 0.73878, 1)))</f>
         <v/>
@@ -12500,7 +12486,7 @@
       <c r="D207" s="3" t="n">
         <v>7.7</v>
       </c>
-      <c r="E207" s="3" t="inlineStr"/>
+      <c r="E207" s="3" t="n"/>
       <c r="F207" s="3">
         <f>IF(B207="common", 4, IF(B207="uncommon", 3, IF(B207="rare", 0.73878, 1)))</f>
         <v/>
@@ -12672,7 +12658,7 @@
       <c r="D210" s="3" t="n">
         <v>27.4</v>
       </c>
-      <c r="E210" s="3" t="inlineStr"/>
+      <c r="E210" s="3" t="n"/>
       <c r="F210" s="3">
         <f>IF(B210="common", 4, IF(B210="uncommon", 3, IF(B210="rare", 0.73878, 1)))</f>
         <v/>
@@ -12830,7 +12816,7 @@
       <c r="D214" s="3" t="n">
         <v>10.54</v>
       </c>
-      <c r="E214" s="3" t="inlineStr"/>
+      <c r="E214" s="3" t="n"/>
       <c r="F214" s="3">
         <f>IF(B214="common", 4, IF(B214="uncommon", 3, IF(B214="rare", 0.73878, 1)))</f>
         <v/>
@@ -12924,7 +12910,7 @@
       <c r="D217" s="3" t="n">
         <v>0.59</v>
       </c>
-      <c r="E217" s="3" t="inlineStr"/>
+      <c r="E217" s="3" t="n"/>
       <c r="F217" s="3">
         <f>IF(B217="common", 4, IF(B217="uncommon", 3, IF(B217="rare", 0.73878, 1)))</f>
         <v/>
@@ -12954,7 +12940,7 @@
       <c r="D218" s="3" t="n">
         <v>1.87</v>
       </c>
-      <c r="E218" s="3" t="inlineStr"/>
+      <c r="E218" s="3" t="n"/>
       <c r="F218" s="3">
         <f>IF(B218="common", 4, IF(B218="uncommon", 3, IF(B218="rare", 0.73878, 1)))</f>
         <v/>
@@ -12984,7 +12970,7 @@
       <c r="D219" s="3" t="n">
         <v>16.15</v>
       </c>
-      <c r="E219" s="3" t="inlineStr"/>
+      <c r="E219" s="3" t="n"/>
       <c r="F219" s="3">
         <f>IF(B219="common", 4, IF(B219="uncommon", 3, IF(B219="rare", 0.73878, 1)))</f>
         <v/>
@@ -13494,7 +13480,7 @@
       <c r="D235" s="3" t="n">
         <v>5.5</v>
       </c>
-      <c r="E235" s="3" t="inlineStr"/>
+      <c r="E235" s="3" t="n"/>
       <c r="F235" s="3">
         <f>IF(B235="common", 4, IF(B235="uncommon", 3, IF(B235="rare", 0.73878, 1)))</f>
         <v/>
@@ -13556,7 +13542,7 @@
       <c r="D237" s="3" t="n">
         <v>0.63</v>
       </c>
-      <c r="E237" s="3" t="inlineStr"/>
+      <c r="E237" s="3" t="n"/>
       <c r="F237" s="3">
         <f>IF(B237="common", 4, IF(B237="uncommon", 3, IF(B237="rare", 0.73878, 1)))</f>
         <v/>
@@ -13586,7 +13572,7 @@
       <c r="D238" s="3" t="n">
         <v>2.59</v>
       </c>
-      <c r="E238" s="3" t="inlineStr"/>
+      <c r="E238" s="3" t="n"/>
       <c r="F238" s="3">
         <f>IF(B238="common", 4, IF(B238="uncommon", 3, IF(B238="rare", 0.73878, 1)))</f>
         <v/>
@@ -13648,7 +13634,7 @@
       <c r="D240" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="E240" s="3" t="inlineStr"/>
+      <c r="E240" s="3" t="n"/>
       <c r="F240" s="3">
         <f>IF(B240="common", 4, IF(B240="uncommon", 3, IF(B240="rare", 0.73878, 1)))</f>
         <v/>
@@ -13678,7 +13664,7 @@
       <c r="D241" s="3" t="n">
         <v>1.73</v>
       </c>
-      <c r="E241" s="3" t="inlineStr"/>
+      <c r="E241" s="3" t="n"/>
       <c r="F241" s="3">
         <f>IF(B241="common", 4, IF(B241="uncommon", 3, IF(B241="rare", 0.73878, 1)))</f>
         <v/>
@@ -13740,7 +13726,7 @@
       <c r="D243" s="3" t="n">
         <v>3.31</v>
       </c>
-      <c r="E243" s="3" t="inlineStr"/>
+      <c r="E243" s="3" t="n"/>
       <c r="F243" s="3">
         <f>IF(B243="common", 4, IF(B243="uncommon", 3, IF(B243="rare", 0.73878, 1)))</f>
         <v/>
@@ -13770,7 +13756,7 @@
       <c r="D244" s="3" t="n">
         <v>6.78</v>
       </c>
-      <c r="E244" s="3" t="inlineStr"/>
+      <c r="E244" s="3" t="n"/>
       <c r="F244" s="3">
         <f>IF(B244="common", 4, IF(B244="uncommon", 3, IF(B244="rare", 0.73878, 1)))</f>
         <v/>
@@ -13832,7 +13818,7 @@
       <c r="D246" s="3" t="n">
         <v>8.6</v>
       </c>
-      <c r="E246" s="3" t="inlineStr"/>
+      <c r="E246" s="3" t="n"/>
       <c r="F246" s="3">
         <f>IF(B246="common", 4, IF(B246="uncommon", 3, IF(B246="rare", 0.73878, 1)))</f>
         <v/>
@@ -13958,7 +13944,7 @@
       <c r="D250" s="3" t="n">
         <v>5.7</v>
       </c>
-      <c r="E250" s="3" t="inlineStr"/>
+      <c r="E250" s="3" t="n"/>
       <c r="F250" s="3">
         <f>IF(B250="common", 4, IF(B250="uncommon", 3, IF(B250="rare", 0.73878, 1)))</f>
         <v/>
@@ -14180,7 +14166,7 @@
       <c r="D257" s="3" t="n">
         <v>5.93</v>
       </c>
-      <c r="E257" s="3" t="inlineStr"/>
+      <c r="E257" s="3" t="n"/>
       <c r="F257" s="3">
         <f>IF(B257="common", 4, IF(B257="uncommon", 3, IF(B257="rare", 0.73878, 1)))</f>
         <v/>
@@ -14370,7 +14356,7 @@
       <c r="D263" s="3" t="n">
         <v>17.65</v>
       </c>
-      <c r="E263" s="3" t="inlineStr"/>
+      <c r="E263" s="3" t="n"/>
       <c r="F263" s="3">
         <f>IF(B263="common", 4, IF(B263="uncommon", 3, IF(B263="rare", 0.73878, 1)))</f>
         <v/>
@@ -21414,7 +21400,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21424,248 +21410,560 @@
   <cols>
     <col width="13" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="13" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="13" bestFit="1" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="12" t="inlineStr">
-        <is>
-          <t>Metric</t>
-        </is>
-      </c>
-      <c r="B1" s="12" t="inlineStr">
+      <c r="A1" s="10" t="inlineStr">
+        <is>
+          <t>Summary Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="10" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="13" t="inlineStr">
+      <c r="A2" s="11" t="inlineStr">
         <is>
           <t>ev_common_total</t>
         </is>
       </c>
-      <c r="B2" s="14" t="n">
+      <c r="B2" s="11" t="n">
         <v>0.2924675324675324</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="13" t="inlineStr">
+      <c r="A3" s="11" t="inlineStr">
         <is>
           <t>ev_uncommon_total</t>
         </is>
       </c>
-      <c r="B3" s="14" t="n">
+      <c r="B3" s="11" t="n">
         <v>0.331551724137931</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="13" t="inlineStr">
+      <c r="A4" s="11" t="inlineStr">
         <is>
           <t>ev_rare_total</t>
         </is>
       </c>
-      <c r="B4" s="14" t="n">
+      <c r="B4" s="11" t="n">
         <v>0.09483950617283952</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="13" t="inlineStr">
+      <c r="A5" s="11" t="inlineStr">
         <is>
           <t>ev_reverse_total</t>
         </is>
       </c>
-      <c r="B5" s="14" t="n">
+      <c r="B5" s="11" t="n">
         <v>0.3494603206988607</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="13" t="inlineStr">
+      <c r="A6" s="11" t="inlineStr">
         <is>
           <t>ev_ace_spec_total</t>
         </is>
       </c>
-      <c r="B6" s="14" t="n">
+      <c r="B6" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="13" t="inlineStr">
+      <c r="A7" s="11" t="inlineStr">
         <is>
           <t>ev_pokeball_total</t>
         </is>
       </c>
-      <c r="B7" s="14" t="n">
+      <c r="B7" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="13" t="inlineStr">
+      <c r="A8" s="11" t="inlineStr">
         <is>
           <t>ev_master_ball_total</t>
         </is>
       </c>
-      <c r="B8" s="14" t="n">
+      <c r="B8" s="11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="13" t="inlineStr">
+      <c r="A9" s="11" t="inlineStr">
         <is>
           <t>ev_IR_total</t>
         </is>
       </c>
-      <c r="B9" s="14" t="n">
+      <c r="B9" s="11" t="n">
         <v>0.9214253393665157</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="13" t="inlineStr">
+      <c r="A10" s="11" t="inlineStr">
         <is>
           <t>ev_SIR_total</t>
         </is>
       </c>
-      <c r="B10" s="14" t="n">
+      <c r="B10" s="11" t="n">
         <v>0.3927949438202247</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="13" t="inlineStr">
+      <c r="A11" s="11" t="inlineStr">
         <is>
           <t>ev_double_rare_total</t>
         </is>
       </c>
-      <c r="B11" s="14" t="n">
+      <c r="B11" s="11" t="n">
         <v>0.20359375</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="13" t="inlineStr">
+      <c r="A12" s="11" t="inlineStr">
         <is>
           <t>ev_hyper_rare_total</t>
         </is>
       </c>
-      <c r="B12" s="14" t="n">
+      <c r="B12" s="11" t="n">
         <v>0.06614583333333333</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="13" t="inlineStr">
+      <c r="A13" s="11" t="inlineStr">
         <is>
           <t>ev_ultra_rare_total</t>
         </is>
       </c>
-      <c r="B13" s="14" t="n">
+      <c r="B13" s="11" t="n">
         <v>0.2068408551068884</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="13" t="inlineStr">
+      <c r="A14" s="11" t="inlineStr">
         <is>
           <t>reverse_multiplier</t>
         </is>
       </c>
-      <c r="B14" s="13" t="n">
+      <c r="B14" s="11" t="n">
         <v>1.889605205381023</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="13" t="inlineStr">
+      <c r="A15" s="11" t="inlineStr">
         <is>
           <t>rare_multiplier</t>
         </is>
       </c>
-      <c r="B15" s="13" t="n">
+      <c r="B15" s="11" t="n">
         <v>0.7666666666666667</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="13" t="inlineStr">
+      <c r="A16" s="11" t="inlineStr">
+        <is>
+          <t>regular_pack_ev_contribution</t>
+        </is>
+      </c>
+      <c r="B16" s="11" t="n">
+        <v>2.859119805104126</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="11" t="inlineStr">
+        <is>
+          <t>god_pack_ev_contribution</t>
+        </is>
+      </c>
+      <c r="B17" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="11" t="inlineStr">
+        <is>
+          <t>demi_god_pack_ev_contribution</t>
+        </is>
+      </c>
+      <c r="B18" s="11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="11" t="inlineStr">
         <is>
           <t>total_manual_ev</t>
         </is>
       </c>
-      <c r="B16" s="13" t="n">
+      <c r="B19" s="11" t="n">
         <v>2.859119805104126</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="13" t="inlineStr">
-        <is>
-          <t>regular_pack_ev_contribution</t>
-        </is>
-      </c>
-      <c r="B17" s="13" t="n">
+    <row r="21">
+      <c r="A21" s="10" t="inlineStr">
+        <is>
+          <t>Results Metric</t>
+        </is>
+      </c>
+      <c r="B21" s="10" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="11" t="inlineStr">
+        <is>
+          <t>total_manual_ev</t>
+        </is>
+      </c>
+      <c r="B22" s="11" t="n">
         <v>2.859119805104126</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="13" t="inlineStr">
-        <is>
-          <t>god_pack_ev_contribution</t>
-        </is>
-      </c>
-      <c r="B18" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="13" t="inlineStr">
-        <is>
-          <t>demi_god_pack_ev_contribution</t>
-        </is>
-      </c>
-      <c r="B19" s="13" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="13" t="inlineStr">
+    <row r="23">
+      <c r="A23" s="11" t="inlineStr">
+        <is>
+          <t>acutal_simulated_ev</t>
+        </is>
+      </c>
+      <c r="B23" s="11" t="n">
+        <v>2.9096855</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="11" t="inlineStr">
+        <is>
+          <t>pack_price</t>
+        </is>
+      </c>
+      <c r="B24" s="11" t="n">
+        <v>6.05</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="11" t="inlineStr">
+        <is>
+          <t>hit_probability_percentage</t>
+        </is>
+      </c>
+      <c r="B25" s="11" t="n">
+        <v>28.37362152609313</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="11" t="inlineStr">
+        <is>
+          <t>no_hit_probability_percentage</t>
+        </is>
+      </c>
+      <c r="B26" s="11" t="n">
+        <v>71.62637847390687</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="11" t="inlineStr">
         <is>
           <t>net_value</t>
         </is>
       </c>
-      <c r="B20" s="14" t="n">
-        <v>-3.1817187</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="13" t="inlineStr">
+      <c r="B27" s="11" t="n">
+        <v>-3.1403145</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="11" t="inlineStr">
         <is>
           <t>opening_pack_roi</t>
         </is>
       </c>
-      <c r="B21" s="13" t="n">
-        <v>0.4740960826446281</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="13" t="inlineStr">
+      <c r="B28" s="11" t="n">
+        <v>0.4809397520661157</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="11" t="inlineStr">
         <is>
           <t>opening_pack_roi_percent</t>
         </is>
       </c>
-      <c r="B22" s="13" t="n">
-        <v>-52.59039173553719</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="13" t="inlineStr">
-        <is>
-          <t>no_hit_probability_percentage</t>
-        </is>
-      </c>
-      <c r="B23" s="15" t="n">
-        <v>0.7162637847390687</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="13" t="inlineStr">
-        <is>
-          <t>hit_probability_percentage</t>
-        </is>
-      </c>
-      <c r="B24" s="15" t="n">
-        <v>0.2837362152609313</v>
+      <c r="B29" s="11" t="n">
+        <v>-51.90602479338844</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="10" t="inlineStr">
+        <is>
+          <t>Simulation Metric</t>
+        </is>
+      </c>
+      <c r="B31" s="10" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Mean Value</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>2.9096855</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Standard Deviation</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>6.442374480119093</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Minimum Value</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Maximum Value</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>104.67</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>5th</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>0.8200000000000001</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>25th</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>50th (median)</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1.09</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>75th</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>90th</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>6.449999999999999</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>95th</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>12.10049999999988</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>99th</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>28.21</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="10" t="inlineStr">
+        <is>
+          <t>Top 10 Most Expensive Hits</t>
+        </is>
+      </c>
+      <c r="B44" s="10" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="C44" s="10" t="inlineStr">
+        <is>
+          <t>Effective Pull Rate</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Groudon - 199/182</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>91.09</v>
+      </c>
+      <c r="C45" t="n">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Roaring Moon ex - 251/182</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>43.85</v>
+      </c>
+      <c r="C46" t="n">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Altaria ex - 253/182</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>43.83</v>
+      </c>
+      <c r="C47" t="n">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Garchomp ex - 245/182</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>34.59</v>
+      </c>
+      <c r="C48" t="n">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Gholdengo ex - 252/182</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>29.93</v>
+      </c>
+      <c r="C49" t="n">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Steelix - 208/182</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>27.4</v>
+      </c>
+      <c r="C50" t="n">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Iron Valiant ex - 249/182</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>23.01</v>
+      </c>
+      <c r="C51" t="n">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Minun - 194/182</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>22.43</v>
+      </c>
+      <c r="C52" t="n">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Plusle - 193/182</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>20.85</v>
+      </c>
+      <c r="C53" t="n">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Morpeko - 206/182</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>20.49</v>
+      </c>
+      <c r="C54" t="n">
+        <v>442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>